<commit_message>
added directory for notebooks_and_demonstration
</commit_message>
<xml_diff>
--- a/fund_statement_extractor/output/pytesseract/final_outputs/flare_extraction_marked.xlsx
+++ b/fund_statement_extractor/output/pytesseract/final_outputs/flare_extraction_marked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinjonany/Desktop/python/data-science/projects/RAG Techniques/FLARE-Implementation/fund_statement_extractor/output/pytesseract/final_outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB0C213-6308-3C40-A9D4-30A25B5EC53D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EA2981-99FD-CD49-A9C6-81FC6BF0DDC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14300" yWindow="500" windowWidth="14500" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -825,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>